<commit_message>
30-11 updated for Created Project TAsked
</commit_message>
<xml_diff>
--- a/titan30/titan/src/test/resources/excel/CreateProject.xlsx
+++ b/titan30/titan/src/test/resources/excel/CreateProject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17505" windowHeight="8040" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17505" windowHeight="8040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewProject" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="49">
   <si>
     <t>ProjectCode</t>
   </si>
@@ -121,9 +121,6 @@
     <t>YT606</t>
   </si>
   <si>
-    <t>YT626</t>
-  </si>
-  <si>
     <t>TaskName</t>
   </si>
   <si>
@@ -148,34 +145,25 @@
     <t>Top</t>
   </si>
   <si>
-    <t>YT627</t>
-  </si>
-  <si>
-    <t>Task06</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jitendra </t>
   </si>
   <si>
-    <t>TeamMember</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
     <t>EngageDate</t>
   </si>
   <si>
     <t>ExRelasedate</t>
   </si>
   <si>
-    <t>Demo1 Titan</t>
-  </si>
-  <si>
-    <t>Developer</t>
-  </si>
-  <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>Demo Titan</t>
+  </si>
+  <si>
+    <t>Task08</t>
+  </si>
+  <si>
+    <t>YTP565</t>
   </si>
 </sst>
 </file>
@@ -232,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -241,7 +229,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -547,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,10 +614,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>25</v>
@@ -657,7 +644,7 @@
         <v>7</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>16</v>
@@ -677,115 +664,6 @@
       <c r="Q2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1041,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,19 +932,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>20</v>
@@ -1074,22 +952,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1100,40 +978,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>52</v>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated extend report on 04-Jan-19
</commit_message>
<xml_diff>
--- a/titan30/titan/src/test/resources/excel/CreateProject.xlsx
+++ b/titan30/titan/src/test/resources/excel/CreateProject.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="62">
   <si>
     <t>ProjectCode</t>
   </si>
@@ -200,7 +200,10 @@
     <t>New Task Create Successfully</t>
   </si>
   <si>
-    <t>POL521</t>
+    <t>ForceFully Failed</t>
+  </si>
+  <si>
+    <t>PROJECT001</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,10 +654,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>25</v>
@@ -957,7 +960,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1069,7 @@
         <v>41</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1112,7 +1115,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>